<commit_message>
Evaporation implemented - nu v/s z verification done
</commit_message>
<xml_diff>
--- a/Archive/Reports/0201 Time analysis for LBM vs MOL.xlsx
+++ b/Archive/Reports/0201 Time analysis for LBM vs MOL.xlsx
@@ -401,6 +401,67 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> v/s Number of points </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -651,6 +712,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of points</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -713,6 +834,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1977,16 +2154,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>643924</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>195648</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>466125</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>94049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2273,8 +2450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="111" zoomScaleNormal="111" zoomScalePageLayoutView="111" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="111" zoomScaleNormal="111" zoomScalePageLayoutView="111" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Test for time comparison of LB and MOL
</commit_message>
<xml_diff>
--- a/Archive/Reports/0201 Time analysis for LBM vs MOL.xlsx
+++ b/Archive/Reports/0201 Time analysis for LBM vs MOL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -215,11 +215,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2115737664"/>
-        <c:axId val="-2123429584"/>
+        <c:axId val="2122180496"/>
+        <c:axId val="2121129056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2115737664"/>
+        <c:axId val="2122180496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -276,12 +276,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2123429584"/>
+        <c:crossAx val="2121129056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2123429584"/>
+        <c:axId val="2121129056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -338,7 +338,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115737664"/>
+        <c:crossAx val="2122180496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -688,11 +688,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2116320496"/>
-        <c:axId val="-2130705664"/>
+        <c:axId val="2082286448"/>
+        <c:axId val="2078537872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2116320496"/>
+        <c:axId val="2082286448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -809,12 +809,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2130705664"/>
+        <c:crossAx val="2078537872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2130705664"/>
+        <c:axId val="2078537872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -927,7 +927,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2116320496"/>
+        <c:crossAx val="2082286448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2154,16 +2154,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>643924</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>195648</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>655366</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>138441</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>466125</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>94049</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>477567</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>36842</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2451,7 +2451,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="111" zoomScaleNormal="111" zoomScalePageLayoutView="111" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2532,7 +2532,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <f t="shared" ref="A7:A15" si="0">4*A6</f>
+        <f t="shared" ref="A7:A9" si="0">4*A6</f>
         <v>409600</v>
       </c>
       <c r="B7">

</xml_diff>